<commit_message>
Changed the cutting code a bit and also some data
</commit_message>
<xml_diff>
--- a/data/2024-05-13_bothslitsIN_grating.xlsx
+++ b/data/2024-05-13_bothslitsIN_grating.xlsx
@@ -132,8 +132,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -164,7 +164,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>3.2E-005</v>
+        <v>2E-005</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>32</v>
@@ -172,7 +172,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>6.9E-005</v>
+        <v>2.8E-005</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>69</v>
@@ -180,7 +180,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>9.4E-005</v>
+        <v>3.6E-005</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>94</v>
@@ -188,7 +188,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>8.8E-005</v>
+        <v>4.4E-005</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>88</v>
@@ -196,7 +196,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>0.000136</v>
+        <v>5.3E-005</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>136</v>
@@ -204,7 +204,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>0.000125</v>
+        <v>6E-005</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>125</v>
@@ -212,7 +212,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>0.000148</v>
+        <v>6.9E-005</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>148</v>
@@ -220,7 +220,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>0.000154</v>
+        <v>8E-005</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>154</v>
@@ -228,7 +228,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>0.000168</v>
+        <v>9E-005</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>168</v>
@@ -236,7 +236,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>0.00015</v>
+        <v>9.9E-005</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>150</v>
@@ -244,7 +244,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>0.00016</v>
+        <v>0.000109</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>160</v>
@@ -252,7 +252,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>0.000157</v>
+        <v>0.000121</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>157</v>

</xml_diff>